<commit_message>
updated user answer ranges and made it (1/2...)
</commit_message>
<xml_diff>
--- a/Code/User_Profile.xlsx
+++ b/Code/User_Profile.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ariadruker/Documents/Northeastern/5800/Final_Project/Code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E84751B-6994-2946-8A60-842B18DBC135}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCB80C0F-95F2-284E-A02F-DF6BE1E7D126}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16100" xr2:uid="{31C34B65-AE2F-5C46-8569-64A4A3E43CF1}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28420" windowHeight="16100" xr2:uid="{31C34B65-AE2F-5C46-8569-64A4A3E43CF1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
   <si>
     <t>Variable</t>
   </si>
@@ -59,9 +59,6 @@
     <t>Time horizon</t>
   </si>
   <si>
-    <t>&gt;20</t>
-  </si>
-  <si>
     <t>years</t>
   </si>
   <si>
@@ -74,18 +71,9 @@
     <t>Fluctuations</t>
   </si>
   <si>
-    <t>&gt;15</t>
-  </si>
-  <si>
-    <t>&gt;10</t>
-  </si>
-  <si>
     <t>Worst case</t>
   </si>
   <si>
-    <t>&gt;35</t>
-  </si>
-  <si>
     <t>Units</t>
   </si>
   <si>
@@ -95,22 +83,28 @@
     <t>Y-Axis</t>
   </si>
   <si>
-    <t>Returns</t>
-  </si>
-  <si>
     <t>X-Axis</t>
   </si>
   <si>
-    <t>Risk</t>
-  </si>
-  <si>
-    <t>dropdown</t>
-  </si>
-  <si>
-    <t>STD</t>
-  </si>
-  <si>
-    <t>Z</t>
+    <t>Metric</t>
+  </si>
+  <si>
+    <t>Window of Data</t>
+  </si>
+  <si>
+    <t>STD Deviation</t>
+  </si>
+  <si>
+    <t>Max Dropdown</t>
+  </si>
+  <si>
+    <t>Filter</t>
+  </si>
+  <si>
+    <t>Function</t>
+  </si>
+  <si>
+    <t>Average Calculation Range</t>
   </si>
 </sst>
 </file>
@@ -488,18 +482,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D4E6B42-C3F2-3848-A254-A541CB2D33C6}">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
+    <col min="8" max="8" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -519,108 +515,105 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" t="s">
         <v>16</v>
       </c>
       <c r="I1" t="s">
-        <v>18</v>
-      </c>
-      <c r="J1" t="s">
-        <v>19</v>
-      </c>
-      <c r="K1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
       <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>4</v>
+      </c>
+      <c r="D2">
+        <v>8</v>
+      </c>
+      <c r="E2">
+        <v>15</v>
+      </c>
+      <c r="F2">
+        <v>25</v>
+      </c>
+      <c r="G2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3">
         <v>2</v>
       </c>
-      <c r="C2">
+      <c r="C3">
+        <v>4</v>
+      </c>
+      <c r="D3">
+        <v>6</v>
+      </c>
+      <c r="E3">
+        <v>8</v>
+      </c>
+      <c r="F3">
+        <v>11</v>
+      </c>
+      <c r="G3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4">
         <v>5</v>
       </c>
-      <c r="D2">
-        <v>10</v>
-      </c>
-      <c r="E2">
-        <v>20</v>
-      </c>
-      <c r="F2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="E4">
         <v>8</v>
       </c>
-      <c r="I2" t="s">
-        <v>20</v>
-      </c>
-      <c r="J2" t="s">
-        <v>21</v>
-      </c>
-      <c r="K2" t="s">
-        <v>22</v>
+      <c r="F4">
+        <v>100</v>
+      </c>
+      <c r="G4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I4" t="s">
+        <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3">
-        <v>3</v>
-      </c>
-      <c r="C3">
-        <v>5</v>
-      </c>
-      <c r="D3">
-        <v>7</v>
-      </c>
-      <c r="E3">
-        <v>9</v>
-      </c>
-      <c r="F3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I3" t="s">
-        <v>24</v>
-      </c>
-      <c r="J3" t="s">
-        <v>21</v>
-      </c>
-      <c r="K3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>11</v>
-      </c>
-      <c r="B4">
-        <v>3</v>
-      </c>
-      <c r="C4">
-        <v>6</v>
-      </c>
-      <c r="D4">
-        <v>10</v>
-      </c>
-      <c r="E4">
-        <v>15</v>
-      </c>
-      <c r="F4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>14</v>
       </c>
       <c r="B5">
         <v>5</v>
@@ -634,11 +627,17 @@
       <c r="E5">
         <v>35</v>
       </c>
-      <c r="F5" t="s">
-        <v>15</v>
+      <c r="F5">
+        <v>100</v>
       </c>
       <c r="G5" t="s">
-        <v>10</v>
+        <v>9</v>
+      </c>
+      <c r="H5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I5" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>